<commit_message>
ajout de la page listant les ateliers de tous les laboratoires + traitement de l'uri dans DetailsAtelierServlet.java
</commit_message>
<xml_diff>
--- a/doc/TP_Genie_log.xlsx
+++ b/doc/TP_Genie_log.xlsx
@@ -1,12 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippediep/Documents/Projects/GenieLog/repo/genieLogicielGRDP/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="24520" windowHeight="15540" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -98,10 +111,6 @@
  le jour, l'heure, nombre de places disponibles, le lieu</t>
   </si>
   <si>
-    <t>L'utilisateur aura accès à un bouton "créer un nouvel atelier" qui le redirigera vers 
-une page ou il pourra remplir toutes les informations nécessaire à la création d'un atelier</t>
-  </si>
-  <si>
     <t>US7</t>
   </si>
   <si>
@@ -109,10 +118,6 @@
   </si>
   <si>
     <t>Important</t>
-  </si>
-  <si>
-    <t>L'utilisateur aura accès à un boutons "mes ateliers" qui le 
-redirigera vers une page listant tous les titres d'ateliers qu'il a créé</t>
   </si>
   <si>
     <t>US8</t>
@@ -394,26 +399,42 @@
 m'inscrire sur le site (mail, mot de 
 passe, prénom, téléphone)</t>
   </si>
+  <si>
+    <t>L'utilisateur aura accès à la liste de ses ateliers créés directement dans la description de son laboratoire</t>
+  </si>
+  <si>
+    <t>L'utilisateur aura accès à un bouton "ajouter un nouvel atelier" qui le redirigera vers 
+une page ou il pourra remplir toutes les informations nécessaire à la création d'un atelier</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-    </font>
-    <font/>
-    <font>
-      <color rgb="FF333333"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -421,7 +442,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -442,6 +463,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -456,6 +478,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -468,6 +491,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -478,6 +502,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -490,80 +515,330 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Bureau">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Bureau">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Bureau">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.71"/>
-    <col customWidth="1" min="2" max="2" width="89.43"/>
-    <col customWidth="1" min="5" max="5" width="10.57"/>
-    <col customWidth="1" min="6" max="6" width="119.86"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="89.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="119.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -591,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -603,7 +878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -611,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -620,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -628,7 +903,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -640,7 +915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -648,7 +923,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -660,7 +935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -668,7 +943,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>23</v>
@@ -678,7 +953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -686,7 +961,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
@@ -694,254 +969,254 @@
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="F10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="9" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="C12" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="F13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="B14" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="12" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="B16" s="13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="C16" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="11" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="C18" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="11" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="B20" s="11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>67</v>
-      </c>
       <c r="C20" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
@@ -950,195 +1225,195 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="11" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="B23" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="C23" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="C25" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="11" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="B27" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="C27" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C29" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="C30" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>7</v>
@@ -1147,92 +1422,92 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C32" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="3" t="s">
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="C33" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
+      <c r="C34" s="5">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="C36" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>